<commit_message>
DB add first solution of constraints table
</commit_message>
<xml_diff>
--- a/S3/DB/Labor/Teil2/Constraints.xlsx
+++ b/S3/DB/Labor/Teil2/Constraints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladb/Git/htwg/S3/DB/Labor/Teil2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31B3653-6FD7-9D41-A1F6-1A4E2D940304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0109F06-B51F-9646-A4E5-E8A44D691DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23580" windowHeight="21140" xr2:uid="{DEC12530-E22E-0949-BA6C-64ED62393C0C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20680" windowHeight="21140" xr2:uid="{DEC12530-E22E-0949-BA6C-64ED62393C0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="116">
   <si>
     <t>Tabelle</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Wohnungsnummer</t>
   </si>
   <si>
-    <t>&lt; 50</t>
-  </si>
-  <si>
     <t>Entfernung in km</t>
   </si>
   <si>
@@ -199,6 +196,192 @@
   </si>
   <si>
     <t>Ausstattung(auname)</t>
+  </si>
+  <si>
+    <t>Bild</t>
+  </si>
+  <si>
+    <t>bildnr</t>
+  </si>
+  <si>
+    <t>Bildnummer</t>
+  </si>
+  <si>
+    <t>pfad</t>
+  </si>
+  <si>
+    <t>Pfad des Bildes</t>
+  </si>
+  <si>
+    <t>Adresse(anr)</t>
+  </si>
+  <si>
+    <t>grosse</t>
+  </si>
+  <si>
+    <t>Name der Wohnung</t>
+  </si>
+  <si>
+    <t>Größe in qm</t>
+  </si>
+  <si>
+    <t>preis</t>
+  </si>
+  <si>
+    <t>Preis pro Tag in Euro</t>
+  </si>
+  <si>
+    <t>anz</t>
+  </si>
+  <si>
+    <t>Anzahl der Zimmer</t>
+  </si>
+  <si>
+    <t>Wohnung</t>
+  </si>
+  <si>
+    <t>&lt;= 50</t>
+  </si>
+  <si>
+    <t>Kunde</t>
+  </si>
+  <si>
+    <t>knr</t>
+  </si>
+  <si>
+    <t>Kundennummer</t>
+  </si>
+  <si>
+    <t>vorname</t>
+  </si>
+  <si>
+    <t>Name vom Kunde</t>
+  </si>
+  <si>
+    <t>Vorname vom Kunde</t>
+  </si>
+  <si>
+    <t>newsletter</t>
+  </si>
+  <si>
+    <t>Hat den Newsletter abonniert?</t>
+  </si>
+  <si>
+    <t>Bool</t>
+  </si>
+  <si>
+    <t>max. 34</t>
+  </si>
+  <si>
+    <t>iban</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bankverbindung</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Mailadresse</t>
+  </si>
+  <si>
+    <t>Buchung</t>
+  </si>
+  <si>
+    <t>bnr</t>
+  </si>
+  <si>
+    <t>Buchungsnummer</t>
+  </si>
+  <si>
+    <t>Kundennumer</t>
+  </si>
+  <si>
+    <t>Kunde(knr)</t>
+  </si>
+  <si>
+    <t>anreise</t>
+  </si>
+  <si>
+    <t>Anreisedatum</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>abreise</t>
+  </si>
+  <si>
+    <t>Abreisedatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abreise - anreise &gt;= 3 </t>
+  </si>
+  <si>
+    <t>&gt;= aktuelles Datum</t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>Buchungsdatum</t>
+  </si>
+  <si>
+    <t>bDatum</t>
+  </si>
+  <si>
+    <t>beDatum</t>
+  </si>
+  <si>
+    <t>Bewertungsdatum</t>
+  </si>
+  <si>
+    <t>Anzahl Sternen</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 &lt; anz </t>
+  </si>
+  <si>
+    <t>rnr</t>
+  </si>
+  <si>
+    <t>Rechnungsnummer</t>
+  </si>
+  <si>
+    <t>rDatum</t>
+  </si>
+  <si>
+    <t>Rechnungsdatum</t>
+  </si>
+  <si>
+    <t>betrag</t>
+  </si>
+  <si>
+    <t>&gt; abreise</t>
+  </si>
+  <si>
+    <t>Rechnungsbetrag</t>
+  </si>
+  <si>
+    <t>Anzahlung</t>
+  </si>
+  <si>
+    <t>annr</t>
+  </si>
+  <si>
+    <t>Anzahlungsnummer</t>
+  </si>
+  <si>
+    <t>Buchung(bnr)</t>
+  </si>
+  <si>
+    <t>Anzahlungsdatum</t>
+  </si>
+  <si>
+    <t>Anzahlungsbetrag</t>
   </si>
 </sst>
 </file>
@@ -550,15 +733,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B53B8C8-2B1D-8A4A-A59B-9EE580906467}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" customWidth="1"/>
@@ -641,7 +824,10 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -827,7 +1013,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -835,7 +1021,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>40</v>
@@ -850,7 +1036,7 @@
         <v>30</v>
       </c>
       <c r="J15" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -861,7 +1047,10 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
@@ -873,7 +1062,7 @@
         <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J16" t="s">
         <v>33</v>
@@ -881,7 +1070,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -902,7 +1091,7 @@
         <v>20</v>
       </c>
       <c r="I17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J17" t="s">
         <v>33</v>
@@ -910,7 +1099,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -918,7 +1107,7 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>19</v>
@@ -938,10 +1127,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
         <v>50</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -952,7 +1141,10 @@
         <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
@@ -964,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J21" t="s">
         <v>33</v>
@@ -972,10 +1164,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
@@ -993,10 +1185,754 @@
         <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J22" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" t="s">
+        <v>44</v>
+      </c>
+      <c r="J41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" t="s">
+        <v>87</v>
+      </c>
+      <c r="J42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" t="s">
+        <v>30</v>
+      </c>
+      <c r="J43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" t="s">
+        <v>30</v>
+      </c>
+      <c r="J44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="F47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" t="s">
+        <v>30</v>
+      </c>
+      <c r="J47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" t="s">
+        <v>101</v>
+      </c>
+      <c r="G48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" t="s">
+        <v>30</v>
+      </c>
+      <c r="J48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" t="s">
+        <v>30</v>
+      </c>
+      <c r="H50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" t="s">
+        <v>21</v>
+      </c>
+      <c r="G51" t="s">
+        <v>30</v>
+      </c>
+      <c r="H51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" t="s">
+        <v>113</v>
+      </c>
+      <c r="J53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+      <c r="F54" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" t="s">
+        <v>21</v>
+      </c>
+      <c r="G55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB finish constrains, user cases and zugriffsmatrix
</commit_message>
<xml_diff>
--- a/S3/DB/Labor/Teil2/Constraints.xlsx
+++ b/S3/DB/Labor/Teil2/Constraints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladb/Git/htwg/S3/DB/Labor/Teil2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0109F06-B51F-9646-A4E5-E8A44D691DD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F465DD-2EEA-4345-9781-F294BFB5BA89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20680" windowHeight="21140" xr2:uid="{DEC12530-E22E-0949-BA6C-64ED62393C0C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{DEC12530-E22E-0949-BA6C-64ED62393C0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="118">
   <si>
     <t>Tabelle</t>
   </si>
@@ -276,9 +276,6 @@
     <t>iban</t>
   </si>
   <si>
-    <t xml:space="preserve"> Bankverbindung</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>k</t>
   </si>
   <si>
-    <t xml:space="preserve">1 &lt; anz </t>
-  </si>
-  <si>
     <t>rnr</t>
   </si>
   <si>
@@ -382,6 +376,18 @@
   </si>
   <si>
     <t>Anzahlungsbetrag</t>
+  </si>
+  <si>
+    <t>1 &lt;= anz &lt;= 5</t>
+  </si>
+  <si>
+    <t>&gt;= 0</t>
+  </si>
+  <si>
+    <t>ON DELETE CASCADE</t>
+  </si>
+  <si>
+    <t>Bankverbindung</t>
   </si>
 </sst>
 </file>
@@ -735,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B53B8C8-2B1D-8A4A-A59B-9EE580906467}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,10 +751,12 @@
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="8.5" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -824,10 +832,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -1047,10 +1052,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
@@ -1065,7 +1067,7 @@
         <v>44</v>
       </c>
       <c r="J16" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1094,7 +1096,7 @@
         <v>46</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1122,7 +1124,7 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1141,10 +1143,7 @@
         <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
@@ -1159,7 +1158,7 @@
         <v>44</v>
       </c>
       <c r="J21" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1188,7 +1187,7 @@
         <v>53</v>
       </c>
       <c r="J22" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1204,10 +1203,7 @@
         <v>56</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F24" t="s">
         <v>21</v>
@@ -1227,10 +1223,7 @@
         <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F25" t="s">
         <v>21</v>
@@ -1245,7 +1238,7 @@
         <v>44</v>
       </c>
       <c r="J25" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1282,10 +1275,7 @@
         <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F27" t="s">
         <v>21</v>
@@ -1305,10 +1295,7 @@
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F28" t="s">
         <v>21</v>
@@ -1420,10 +1407,7 @@
         <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F33" t="s">
         <v>21</v>
@@ -1443,10 +1427,7 @@
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
         <v>21</v>
@@ -1535,7 +1516,7 @@
         <v>79</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="D38" t="s">
         <v>19</v>
@@ -1555,10 +1536,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
         <v>81</v>
-      </c>
-      <c r="C39" t="s">
-        <v>82</v>
       </c>
       <c r="D39" t="s">
         <v>19</v>
@@ -1578,19 +1559,16 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
         <v>83</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>84</v>
       </c>
-      <c r="C40" t="s">
-        <v>85</v>
-      </c>
       <c r="D40" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F40" t="s">
         <v>21</v>
@@ -1610,10 +1588,7 @@
         <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F41" t="s">
         <v>21</v>
@@ -1636,25 +1611,22 @@
         <v>70</v>
       </c>
       <c r="C42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" t="s">
         <v>86</v>
-      </c>
-      <c r="D42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42">
-        <v>3</v>
-      </c>
-      <c r="F42" t="s">
-        <v>21</v>
-      </c>
-      <c r="G42" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" t="s">
-        <v>30</v>
-      </c>
-      <c r="I42" t="s">
-        <v>87</v>
       </c>
       <c r="J42" t="s">
         <v>33</v>
@@ -1662,14 +1634,14 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
         <v>88</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>89</v>
       </c>
-      <c r="D43" t="s">
-        <v>90</v>
-      </c>
       <c r="F43" t="s">
         <v>21</v>
       </c>
@@ -1680,18 +1652,18 @@
         <v>30</v>
       </c>
       <c r="J43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
         <v>91</v>
       </c>
-      <c r="C44" t="s">
-        <v>92</v>
-      </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F44" t="s">
         <v>21</v>
@@ -1703,23 +1675,23 @@
         <v>30</v>
       </c>
       <c r="J44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F46" t="s">
         <v>21</v>
@@ -1733,16 +1705,16 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" t="s">
         <v>98</v>
       </c>
-      <c r="C47" t="s">
-        <v>99</v>
-      </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G47" t="s">
         <v>30</v>
@@ -1751,7 +1723,7 @@
         <v>30</v>
       </c>
       <c r="J47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -1759,13 +1731,13 @@
         <v>65</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48" t="s">
         <v>29</v>
       </c>
       <c r="F48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G48" t="s">
         <v>30</v>
@@ -1774,24 +1746,21 @@
         <v>30</v>
       </c>
       <c r="J48" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F49" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="G49" t="s">
         <v>20</v>
@@ -1802,16 +1771,16 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F50" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="G50" t="s">
         <v>30</v>
@@ -1822,39 +1791,39 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s">
         <v>107</v>
-      </c>
-      <c r="C51" t="s">
-        <v>109</v>
       </c>
       <c r="D51" t="s">
         <v>40</v>
       </c>
       <c r="F51" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="G51" t="s">
         <v>30</v>
       </c>
       <c r="H51" t="s">
         <v>30</v>
+      </c>
+      <c r="J51" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" t="s">
         <v>110</v>
       </c>
-      <c r="B52" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" t="s">
-        <v>112</v>
-      </c>
       <c r="D52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F52" t="s">
         <v>21</v>
@@ -1868,16 +1837,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" t="s">
         <v>84</v>
       </c>
-      <c r="C53" t="s">
-        <v>85</v>
-      </c>
       <c r="D53" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="F53" t="s">
         <v>21</v>
@@ -1886,10 +1852,10 @@
         <v>30</v>
       </c>
       <c r="H53" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I53" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J53" t="s">
         <v>33</v>
@@ -1897,13 +1863,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F54" t="s">
         <v>21</v>
@@ -1912,15 +1878,15 @@
         <v>30</v>
       </c>
       <c r="H54" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D55" t="s">
         <v>40</v>
@@ -1937,5 +1903,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DB finish teil 2 and start teil 3
</commit_message>
<xml_diff>
--- a/S3/DB/Labor/Teil2/Constraints.xlsx
+++ b/S3/DB/Labor/Teil2/Constraints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladb/Git/htwg/S3/DB/Labor/Teil2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F465DD-2EEA-4345-9781-F294BFB5BA89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CD652D-770B-B549-B0DC-021A940D376F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{DEC12530-E22E-0949-BA6C-64ED62393C0C}"/>
   </bookViews>
@@ -739,10 +739,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B53B8C8-2B1D-8A4A-A59B-9EE580906467}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1301,7 +1304,7 @@
         <v>21</v>
       </c>
       <c r="G28" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H28" t="s">
         <v>30</v>
@@ -1903,6 +1906,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>